<commit_message>
Adding each training time and the average to the results
</commit_message>
<xml_diff>
--- a/DoS_Detection/results/all_results.xlsx
+++ b/DoS_Detection/results/all_results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="96">
   <si>
     <t>Algorithm</t>
   </si>
@@ -95,6 +95,29 @@
     <t>ALL</t>
   </si>
   <si>
+    <t>24.06753182411194</t>
+  </si>
+  <si>
+    <t>27.17899513244629</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>Average:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> 27.4602467219</t>
+    </r>
+  </si>
+  <si>
     <t>CatBoost</t>
   </si>
   <si>
@@ -102,6 +125,29 @@
   </si>
   <si>
     <t>285.78365659713745</t>
+  </si>
+  <si>
+    <t>271.36679315567017</t>
+  </si>
+  <si>
+    <t>268.5161793231964</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>Average:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> 275.222209692</t>
+    </r>
   </si>
   <si>
     <t>LightGBM</t>
@@ -117,6 +163,29 @@
     <t>5.430677175521851</t>
   </si>
   <si>
+    <t>5.0015716552734375</t>
+  </si>
+  <si>
+    <t>4.982242584228516</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>Average:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> 5.13816380501</t>
+    </r>
+  </si>
+  <si>
     <t>LightGBM (with BO)</t>
   </si>
   <si>
@@ -128,6 +197,29 @@
   </si>
   <si>
     <t>6.905789136886597</t>
+  </si>
+  <si>
+    <t>6.514970779418945</t>
+  </si>
+  <si>
+    <t>6.629354953765869</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>Average:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> 6.68337162336</t>
+    </r>
   </si>
   <si>
     <t>0.97</t>
@@ -544,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -573,6 +665,9 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="9" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
@@ -581,6 +676,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -832,7 +933,7 @@
     <col customWidth="1" min="5" max="5" width="11.63"/>
     <col customWidth="1" min="6" max="6" width="12.63"/>
     <col customWidth="1" min="7" max="7" width="19.5"/>
-    <col customWidth="1" min="8" max="8" width="24.0"/>
+    <col customWidth="1" min="8" max="8" width="37.88"/>
     <col customWidth="1" min="9" max="9" width="17.75"/>
   </cols>
   <sheetData>
@@ -907,57 +1008,44 @@
       <c r="G3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="15" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="11"/>
       <c r="L3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="15"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="16"/>
       <c r="J4" s="11"/>
       <c r="L4" s="12"/>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="13" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="15"/>
+      <c r="I5" s="16"/>
       <c r="J5" s="11"/>
       <c r="L5" s="12"/>
-      <c r="M5" s="16"/>
     </row>
     <row r="6">
       <c r="A6" s="8"/>
@@ -967,8 +1055,10 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="15"/>
+      <c r="H6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="16"/>
       <c r="J6" s="11"/>
       <c r="L6" s="12"/>
     </row>
@@ -992,140 +1082,117 @@
         <v>21</v>
       </c>
       <c r="G7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="15"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="11"/>
       <c r="L7" s="12"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="15"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="16"/>
       <c r="J8" s="11"/>
       <c r="L8" s="12"/>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="15"/>
+      <c r="I9" s="16"/>
       <c r="J9" s="11"/>
       <c r="L9" s="12"/>
     </row>
     <row r="10">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="16"/>
       <c r="J10" s="11"/>
       <c r="L10" s="12"/>
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="H11" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="I11" s="16"/>
       <c r="J11" s="11"/>
       <c r="L11" s="12"/>
     </row>
     <row r="12">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="15"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="16"/>
       <c r="J12" s="11"/>
       <c r="L12" s="12"/>
     </row>
     <row r="13">
-      <c r="A13" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="15"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="16"/>
       <c r="J13" s="11"/>
       <c r="L13" s="12"/>
     </row>
@@ -1137,92 +1204,84 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="15"/>
+      <c r="H14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="16"/>
       <c r="J14" s="11"/>
       <c r="L14" s="12"/>
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="15"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="11"/>
       <c r="L15" s="12"/>
     </row>
     <row r="16">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="15"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="16"/>
       <c r="J16" s="11"/>
       <c r="L16" s="12"/>
     </row>
     <row r="17">
-      <c r="A17" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="15"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="16"/>
       <c r="J17" s="11"/>
       <c r="L17" s="12"/>
     </row>
     <row r="18">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="18"/>
       <c r="J18" s="11"/>
       <c r="L18" s="12"/>
     </row>
@@ -1231,28 +1290,28 @@
         <v>11</v>
       </c>
       <c r="B19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="13" t="s">
+      <c r="H19" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="I19" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="J19" s="11"/>
       <c r="L19" s="12"/>
@@ -1266,36 +1325,36 @@
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="15"/>
+      <c r="I20" s="16"/>
       <c r="J20" s="11"/>
       <c r="L20" s="12"/>
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G21" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="I21" s="15"/>
+      <c r="I21" s="16"/>
       <c r="J21" s="11"/>
       <c r="L21" s="12"/>
     </row>
@@ -1308,36 +1367,36 @@
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="15"/>
+      <c r="I22" s="16"/>
       <c r="J22" s="11"/>
       <c r="L22" s="12"/>
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F23" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="H23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="I23" s="15"/>
+      <c r="I23" s="16"/>
       <c r="J23" s="11"/>
       <c r="L23" s="12"/>
     </row>
@@ -1350,49 +1409,49 @@
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="15"/>
+      <c r="I24" s="16"/>
       <c r="J24" s="11"/>
       <c r="L24" s="12"/>
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="H25" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H25" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="I25" s="15"/>
+      <c r="I25" s="16"/>
       <c r="J25" s="11"/>
       <c r="L25" s="12"/>
     </row>
     <row r="26">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
       <c r="J26" s="11"/>
       <c r="L26" s="12"/>
     </row>
@@ -1401,28 +1460,28 @@
         <v>11</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27" s="14" t="s">
         <v>57</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="J27" s="11"/>
       <c r="L27" s="12"/>
@@ -1436,28 +1495,28 @@
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
-      <c r="I28" s="15"/>
+      <c r="I28" s="16"/>
       <c r="J28" s="11"/>
       <c r="L28" s="12"/>
     </row>
     <row r="29">
       <c r="A29" s="13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>59</v>
@@ -1465,7 +1524,7 @@
       <c r="H29" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I29" s="15"/>
+      <c r="I29" s="16"/>
       <c r="J29" s="11"/>
       <c r="L29" s="12"/>
     </row>
@@ -1478,25 +1537,25 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="15"/>
+      <c r="I30" s="16"/>
       <c r="J30" s="11"/>
       <c r="L30" s="12"/>
     </row>
     <row r="31">
       <c r="A31" s="13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F31" s="13" t="s">
         <v>61</v>
@@ -1507,7 +1566,7 @@
       <c r="H31" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I31" s="15"/>
+      <c r="I31" s="16"/>
       <c r="J31" s="11"/>
       <c r="L31" s="12"/>
     </row>
@@ -1520,25 +1579,25 @@
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
-      <c r="I32" s="15"/>
+      <c r="I32" s="16"/>
       <c r="J32" s="11"/>
       <c r="L32" s="12"/>
     </row>
     <row r="33">
       <c r="A33" s="13" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F33" s="13" t="s">
         <v>64</v>
@@ -1549,20 +1608,20 @@
       <c r="H33" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="I33" s="15"/>
+      <c r="I33" s="16"/>
       <c r="J33" s="11"/>
       <c r="L33" s="12"/>
     </row>
     <row r="34">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
       <c r="J34" s="11"/>
       <c r="L34" s="12"/>
     </row>
@@ -1571,19 +1630,19 @@
         <v>11</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>67</v>
@@ -1591,7 +1650,7 @@
       <c r="H35" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I35" s="14" t="s">
+      <c r="I35" s="15" t="s">
         <v>69</v>
       </c>
       <c r="J35" s="11"/>
@@ -1606,36 +1665,36 @@
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="15"/>
+      <c r="I36" s="16"/>
       <c r="J36" s="11"/>
       <c r="L36" s="12"/>
     </row>
     <row r="37">
       <c r="A37" s="13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I37" s="15"/>
+        <v>72</v>
+      </c>
+      <c r="I37" s="16"/>
       <c r="J37" s="11"/>
       <c r="L37" s="12"/>
     </row>
@@ -1648,36 +1707,36 @@
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
-      <c r="I38" s="15"/>
+      <c r="I38" s="16"/>
       <c r="J38" s="11"/>
       <c r="L38" s="12"/>
     </row>
     <row r="39">
       <c r="A39" s="13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="I39" s="15"/>
+        <v>75</v>
+      </c>
+      <c r="I39" s="16"/>
       <c r="J39" s="11"/>
       <c r="L39" s="12"/>
     </row>
@@ -1690,120 +1749,377 @@
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
-      <c r="I40" s="15"/>
+      <c r="I40" s="16"/>
       <c r="J40" s="11"/>
       <c r="L40" s="12"/>
     </row>
     <row r="41">
       <c r="A41" s="13" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="I41" s="15"/>
+        <v>78</v>
+      </c>
+      <c r="I41" s="16"/>
       <c r="J41" s="11"/>
       <c r="L41" s="12"/>
     </row>
     <row r="42">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="20"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="11"/>
+      <c r="L42" s="12"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J43" s="11"/>
+      <c r="L43" s="12"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="11"/>
+      <c r="L44" s="12"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I45" s="16"/>
+      <c r="J45" s="11"/>
+      <c r="L45" s="12"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="11"/>
+      <c r="L46" s="12"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I47" s="16"/>
+      <c r="J47" s="11"/>
+      <c r="L47" s="12"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="11"/>
+      <c r="L48" s="12"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I49" s="16"/>
+      <c r="J49" s="11"/>
+      <c r="L49" s="12"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="169">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
+  <mergeCells count="165">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:L50"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="I43:I50"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B3:B6"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="I35:I42"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="J1:L42"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I27:I34"/>
-    <mergeCell ref="C3:C4"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="C29:C30"/>
-    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="I3:I18"/>
+    <mergeCell ref="I19:I26"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="E35:E36"/>
     <mergeCell ref="F35:F36"/>
     <mergeCell ref="G35:G36"/>
     <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I42"/>
     <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="I27:I34"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="D39:D40"/>
@@ -1811,103 +2127,12 @@
     <mergeCell ref="F39:F40"/>
     <mergeCell ref="G39:G40"/>
     <mergeCell ref="H39:H40"/>
+    <mergeCell ref="B41:B42"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="I3:I10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="I11:I18"/>
-    <mergeCell ref="I19:I26"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1924,23 +2149,23 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="21" t="s">
-        <v>78</v>
+      <c r="A1" s="24" t="s">
+        <v>90</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="22" t="s">
-        <v>79</v>
+      <c r="E1" s="25" t="s">
+        <v>91</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="7"/>
     </row>
     <row r="2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24" t="s">
-        <v>80</v>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27" t="s">
+        <v>92</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
@@ -1948,35 +2173,35 @@
       <c r="H2" s="12"/>
     </row>
     <row r="3">
-      <c r="A3" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>83</v>
+      <c r="A3" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>95</v>
       </c>
       <c r="E3" s="11"/>
       <c r="H3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="15"/>
-      <c r="B4" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="A4" s="16"/>
+      <c r="B4" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="15">
         <v>539556.0</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="15">
         <v>863.0</v>
       </c>
       <c r="E4" s="11"/>
       <c r="H4" s="12"/>
     </row>
     <row r="5">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1984,14 +2209,14 @@
       <c r="H5" s="12"/>
     </row>
     <row r="6">
-      <c r="A6" s="15"/>
-      <c r="B6" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="14">
+      <c r="A6" s="16"/>
+      <c r="B6" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="15">
         <v>439.0</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="15">
         <v>13710.0</v>
       </c>
       <c r="E6" s="11"/>
@@ -2002,112 +2227,112 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8">
-      <c r="A8" s="21" t="s">
-        <v>32</v>
+      <c r="A8" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="21" t="s">
-        <v>46</v>
+      <c r="E8" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24" t="s">
-        <v>80</v>
+      <c r="A9" s="26"/>
+      <c r="B9" s="27" t="s">
+        <v>92</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24" t="s">
-        <v>80</v>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27" t="s">
+        <v>92</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>83</v>
+      <c r="A10" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="15"/>
-      <c r="B11" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="14">
+      <c r="A11" s="16"/>
+      <c r="B11" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="15">
         <v>538721.0</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="15">
         <v>1698.0</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" s="14">
+      <c r="E11" s="16"/>
+      <c r="F11" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="15">
         <v>537107.0</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="15">
         <v>3312.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
     <row r="13">
-      <c r="A13" s="15"/>
-      <c r="B13" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="14">
+      <c r="A13" s="16"/>
+      <c r="B13" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="15">
         <v>1820.0</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="15">
         <v>12329.0</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G13" s="14">
+      <c r="E13" s="16"/>
+      <c r="F13" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="15">
         <v>3087.0</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="15">
         <v>11062.0</v>
       </c>
     </row>
@@ -2122,106 +2347,106 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15">
-      <c r="A15" s="21" t="s">
-        <v>57</v>
+      <c r="A15" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="21" t="s">
-        <v>69</v>
+      <c r="E15" s="24" t="s">
+        <v>81</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24" t="s">
-        <v>80</v>
+      <c r="A16" s="26"/>
+      <c r="B16" s="27" t="s">
+        <v>92</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="24" t="s">
-        <v>80</v>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27" t="s">
+        <v>92</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>83</v>
+      <c r="A17" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="26"/>
+      <c r="G17" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="15"/>
-      <c r="B18" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="14">
+      <c r="A18" s="16"/>
+      <c r="B18" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="15">
         <v>537595.0</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="15">
         <v>2824.0</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="G18" s="14">
+      <c r="E18" s="16"/>
+      <c r="F18" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="15">
         <v>537658.0</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="15">
         <v>2761.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="15"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="15"/>
+      <c r="E19" s="16"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
     <row r="20">
-      <c r="A20" s="15"/>
-      <c r="B20" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="14">
+      <c r="A20" s="16"/>
+      <c r="B20" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="15">
         <v>3087.0</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="15">
         <v>11062.0</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" s="14">
+      <c r="E20" s="16"/>
+      <c r="F20" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="15">
         <v>3087.0</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="15">
         <v>11062.0</v>
       </c>
     </row>

</xml_diff>